<commit_message>
Editando el archivo excel desde la rama web
</commit_message>
<xml_diff>
--- a/Ex1.xlsx
+++ b/Ex1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\trabajos generales\Lenguaje de programacion 2\Teoria\Clase marzo 24 y 29\repo2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3F3BB1-42A0-4B78-81B2-4551B1A569B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F4FAEB-6D8E-4D06-90B8-4AF9788013FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30" yWindow="3240" windowWidth="17340" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3240" windowWidth="17340" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -345,10 +345,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,6 +388,11 @@
         <v>16</v>
       </c>
     </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>